<commit_message>
Network Contact List 2.0
</commit_message>
<xml_diff>
--- a/manage-network-contacts.xlsx
+++ b/manage-network-contacts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peytonhaws/Documents/Professional Readiness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35FC89-2CD7-3249-9FF2-136D5DEF6A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C40656-F4AD-574D-9D55-C9F2853D2E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{AE6EC594-1444-43B3-9AD5-706BE80652EF}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="189">
   <si>
     <t>(111) 111-1111</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Future Plan</t>
   </si>
   <si>
-    <t>Friends &amp; Family</t>
-  </si>
-  <si>
     <t>Angela</t>
   </si>
   <si>
@@ -265,6 +262,351 @@
   </si>
   <si>
     <t>millardr@byui.edu</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandon </t>
+  </si>
+  <si>
+    <t>Thornton</t>
+  </si>
+  <si>
+    <t>406-925-1081</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Marlynn</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>406-560-2771</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Janet</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Ransom</t>
+  </si>
+  <si>
+    <t>816-698-2318</t>
+  </si>
+  <si>
+    <t>jransom@burnsmcd.com</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike </t>
+  </si>
+  <si>
+    <t>Pond</t>
+  </si>
+  <si>
+    <t>pondmike@niatec.isu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex </t>
+  </si>
+  <si>
+    <t>Nielson</t>
+  </si>
+  <si>
+    <t>nielalex@niatech.isu.edu</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Ratelle</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>Mueller</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Dummar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh </t>
+  </si>
+  <si>
+    <t>Phillips</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Lopata</t>
+  </si>
+  <si>
+    <t>Seth</t>
+  </si>
+  <si>
+    <t>Hartman</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Brenton</t>
+  </si>
+  <si>
+    <t>Trebilcock</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Dass</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Robison</t>
+  </si>
+  <si>
+    <t>Brendon</t>
+  </si>
+  <si>
+    <t>Marques</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Westover</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Matos</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Benavides</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Hsu</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Gay</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Longhurst</t>
+  </si>
+  <si>
+    <t>Thieme</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Burr</t>
+  </si>
+  <si>
+    <t>Preston</t>
+  </si>
+  <si>
+    <t>Hon</t>
+  </si>
+  <si>
+    <t>Ison</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>Guilherme</t>
+  </si>
+  <si>
+    <t>Faccinetto</t>
+  </si>
+  <si>
+    <t>Filipe</t>
+  </si>
+  <si>
+    <t>Ferreira</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>Roberts</t>
+  </si>
+  <si>
+    <t>Harrington Jr</t>
+  </si>
+  <si>
+    <t>Glory</t>
+  </si>
+  <si>
+    <t>Ozonuwe</t>
+  </si>
+  <si>
+    <t>Marjorie</t>
+  </si>
+  <si>
+    <t>Brandan</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Doersten</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
+    <t>Guevara</t>
+  </si>
+  <si>
+    <t>Eddy</t>
+  </si>
+  <si>
+    <t>Alfonso</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Skiles</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Malin</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>Waisath</t>
+  </si>
+  <si>
+    <t>Tanner</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>McHatton</t>
+  </si>
+  <si>
+    <t>Camron</t>
+  </si>
+  <si>
+    <t>Thackeray</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Okerlund</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Shirley</t>
+  </si>
+  <si>
+    <t>Larson</t>
+  </si>
+  <si>
+    <t>Vlad</t>
+  </si>
+  <si>
+    <t>Kazandzhi</t>
+  </si>
+  <si>
+    <t>Gamaliel</t>
+  </si>
+  <si>
+    <t>Ortiz</t>
+  </si>
+  <si>
+    <t>Alyssa</t>
+  </si>
+  <si>
+    <t>Kucharyski</t>
+  </si>
+  <si>
+    <t>Kopaunik</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Tipton</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>Jenaca</t>
+  </si>
+  <si>
+    <t>Willans</t>
+  </si>
+  <si>
+    <t>Olsen</t>
   </si>
 </sst>
 </file>
@@ -351,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,9 +742,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1832,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571E2C69-B535-404D-9A63-53D67EC32119}">
-  <dimension ref="A7:H21"/>
+  <dimension ref="A7:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1866,326 +2205,1146 @@
         <v>8</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="18">
         <v>1</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="H8" s="18" t="s">
         <v>23</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="18">
         <v>2</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="F9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="18">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="G10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="18" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="18">
+        <v>4</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="18">
+        <v>5</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="18">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="18">
+        <v>7</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="18">
+        <v>8</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="18">
+        <v>9</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="18">
+        <v>10</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="18">
+        <v>11</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="18">
+        <v>12</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="18">
+        <v>13</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="18">
+        <v>14</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="18">
+        <v>15</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="18">
+        <v>16</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="18">
+        <v>17</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="18">
+        <v>18</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="18">
+        <v>19</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="18">
+        <v>20</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="18">
+        <v>21</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="18">
+        <v>22</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="18">
         <v>23</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="C30" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="18">
+        <v>24</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="18">
+        <v>25</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="18">
+        <v>26</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="18">
+        <v>27</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="18">
+        <v>28</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="18">
+        <v>29</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="18">
+        <v>30</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="18">
+        <v>31</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="18">
+        <v>32</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="18">
+        <v>33</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="18">
+        <v>34</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="18">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="20">
-        <v>4</v>
-      </c>
-      <c r="C11" s="18" t="s">
+      <c r="C42" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="18">
         <v>36</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="C43" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="18">
         <v>37</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="C44" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="18">
         <v>38</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="20" t="s">
+      <c r="C45" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="18">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="20">
-        <v>5</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="C46" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="18">
         <v>40</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="C47" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="18">
         <v>41</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="20" t="s">
+      <c r="C48" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="18">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="20">
-        <v>6</v>
-      </c>
-      <c r="C13" s="20" t="s">
+      <c r="C49" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="18">
         <v>43</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="20" t="s">
+      <c r="C50" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="18">
         <v>44</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="20" t="s">
+      <c r="C51" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="18">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="20">
-        <v>7</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="C52" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="18">
         <v>46</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="20" t="s">
+      <c r="C53" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="18">
         <v>47</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="20" t="s">
+      <c r="C54" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="18">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="20">
-        <v>8</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="C55" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="18">
         <v>49</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="C56" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="18">
         <v>50</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="C57" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="18">
         <v>51</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="20" t="s">
+      <c r="C58" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="18">
+        <v>52</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="18">
+        <v>53</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="18">
+        <v>54</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="18">
+        <v>55</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="18">
+        <v>56</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="18">
+        <v>57</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="18">
+        <v>58</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="18">
+        <v>59</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="18">
+        <v>60</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="18">
+        <v>61</v>
+      </c>
+      <c r="C68" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="20">
-        <v>9</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="20">
-        <v>10</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="20">
-        <v>11</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="20">
-        <v>12</v>
-      </c>
-      <c r="C19" s="20" t="s">
+      <c r="D68" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="18">
         <v>62</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="C69" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="18">
         <v>63</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="C70" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" s="18">
         <v>64</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="C71" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="18">
         <v>65</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="C72" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="18">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="20">
-        <v>13</v>
-      </c>
-      <c r="C20" s="20" t="s">
+      <c r="C73" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="18">
         <v>67</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="C74" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="18">
         <v>68</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="C75" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="18">
         <v>69</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="C76" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="18">
         <v>70</v>
       </c>
-      <c r="G20" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="20">
-        <v>14</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>66</v>
+      <c r="C77" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2196,6 +3355,9 @@
     <hyperlink ref="F19" r:id="rId4" display="mailto:schoendorferf@byui.edu" xr:uid="{93A41E6E-864D-4E4D-A41B-DF9097633130}"/>
     <hyperlink ref="F20" r:id="rId5" display="mailto:masonj@byui.edu" xr:uid="{6F926041-9ABF-3645-ABA4-F5F3D46BB065}"/>
     <hyperlink ref="F21" r:id="rId6" display="mailto:millardr@byui.edu" xr:uid="{FCE29A87-B45E-CC4D-B0B6-6993AB3FA07A}"/>
+    <hyperlink ref="F25" r:id="rId7" xr:uid="{FE3D4D39-9C0F-774E-8FBA-866DBCDCD92D}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{61A9F17B-AA40-9940-8472-C600EB21394A}"/>
+    <hyperlink ref="F27" r:id="rId9" xr:uid="{32816148-FC98-0143-8B2D-0A492026AF15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>